<commit_message>
Updated HELLO to be COMMAND 1
</commit_message>
<xml_diff>
--- a/Research/Line6_Spider_V_USB_Protocol.xlsx
+++ b/Research/Line6_Spider_V_USB_Protocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Packets" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="100">
   <si>
     <t>Introduction</t>
   </si>
@@ -51,9 +51,6 @@
     <t>The ALL INFO packets happen on first connection, It's assumed that these are requesting ALL the information from the Spider V Amp (settings for all the options). It is not required to send these.  </t>
   </si>
   <si>
-    <t>Before every COMMAND the HELLO packet must be sent.  Assuming this is a “Hey, I'm about to send you a command”.</t>
-  </si>
-  <si>
     <t>Also (most importantly), all the data sent from the Spider V amp must be read / acknowledged or it will refuse to listen to commands.  Basically, make sure to read from the USB BULK IN pipe.</t>
   </si>
   <si>
@@ -72,19 +69,19 @@
     <t>...first command</t>
   </si>
   <si>
-    <t>3. HELLO</t>
-  </si>
-  <si>
-    <t>4. CONTROL</t>
+    <t>3. CONTROL 1</t>
+  </si>
+  <si>
+    <t>4. CONTROL 2</t>
   </si>
   <si>
     <t>…for every new command</t>
   </si>
   <si>
-    <t>n. HELLO</t>
-  </si>
-  <si>
-    <t>N+1. CONTROL</t>
+    <t>n. CONTROL 1</t>
+  </si>
+  <si>
+    <t>N+1. CONTROL 2</t>
   </si>
   <si>
     <t>PACKET 1 – CONNECT</t>
@@ -105,10 +102,10 @@
     <t>ALL INFO 2</t>
   </si>
   <si>
-    <t>PACKET 1 - HELLO</t>
-  </si>
-  <si>
-    <t>PACKET 2 - CONTROL</t>
+    <t>PACKET 1 – CONTROL 1</t>
+  </si>
+  <si>
+    <t>PACKET 2 – CONTROL 2</t>
   </si>
   <si>
     <t>f0</t>
@@ -750,8 +747,8 @@
   </sheetPr>
   <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -858,26 +855,24 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="Q13" s="6"/>
       <c r="S13" s="6"/>
     </row>
     <row r="14" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q14" s="6"/>
       <c r="S14" s="6"/>
     </row>
     <row r="15" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0"/>
       <c r="Q15" s="6"/>
       <c r="S15" s="6"/>
     </row>
     <row r="16" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q16" s="6"/>
       <c r="S16" s="6"/>
@@ -889,110 +884,111 @@
     </row>
     <row r="18" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q18" s="6"/>
       <c r="S18" s="6"/>
     </row>
     <row r="19" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q19" s="6"/>
       <c r="S19" s="6"/>
     </row>
     <row r="20" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q20" s="6"/>
       <c r="S20" s="6"/>
     </row>
     <row r="21" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q21" s="6"/>
       <c r="S21" s="6"/>
     </row>
     <row r="22" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q22" s="6"/>
       <c r="S22" s="6"/>
     </row>
     <row r="23" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q23" s="6"/>
       <c r="S23" s="6"/>
     </row>
     <row r="24" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q24" s="6"/>
       <c r="S24" s="6"/>
     </row>
     <row r="25" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q25" s="6"/>
       <c r="S25" s="6"/>
     </row>
     <row r="26" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q26" s="6"/>
       <c r="S26" s="6"/>
     </row>
     <row r="27" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0"/>
       <c r="Q27" s="6"/>
       <c r="S27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L28" s="9"/>
       <c r="M28" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N28" s="9"/>
       <c r="O28" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P28" s="9"/>
       <c r="Q28" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R28" s="9"/>
       <c r="S28" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T28" s="0"/>
     </row>
@@ -1038,47 +1034,47 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>32</v>
       </c>
       <c r="D30" s="0"/>
       <c r="E30" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F30" s="0"/>
       <c r="G30" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J30" s="13"/>
       <c r="K30" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L30" s="13"/>
       <c r="M30" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N30" s="13"/>
       <c r="O30" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P30" s="3"/>
       <c r="Q30" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R30" s="0"/>
       <c r="S30" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="14" t="n">
         <v>0</v>
@@ -1118,7 +1114,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="14" t="n">
         <v>1</v>
@@ -1201,38 +1197,38 @@
         <v>6</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34" s="0"/>
       <c r="E34" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F34" s="0"/>
       <c r="G34" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J34" s="13"/>
       <c r="K34" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L34" s="13"/>
       <c r="M34" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N34" s="13"/>
       <c r="O34" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P34" s="3"/>
       <c r="Q34" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R34" s="0"/>
       <c r="S34" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T34" s="0"/>
     </row>
@@ -1278,7 +1274,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C36" s="14" t="n">
         <v>0</v>
@@ -1356,44 +1352,44 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="16" t="s">
         <v>37</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>38</v>
       </c>
       <c r="D38" s="0"/>
       <c r="E38" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F38" s="0"/>
       <c r="G38" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J38" s="13"/>
       <c r="K38" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L38" s="13"/>
       <c r="M38" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N38" s="13"/>
       <c r="O38" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P38" s="3"/>
       <c r="Q38" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R38" s="0"/>
       <c r="S38" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="T38" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="T38" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1426,14 +1422,14 @@
       </c>
       <c r="P39" s="3"/>
       <c r="Q39" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R39" s="0"/>
       <c r="S39" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="T39" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="T39" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1466,14 +1462,14 @@
       </c>
       <c r="P40" s="3"/>
       <c r="Q40" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R40" s="0"/>
       <c r="S40" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="T40" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="T40" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,20 +1612,20 @@
       </c>
       <c r="N44" s="3"/>
       <c r="O44" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P44" s="3"/>
       <c r="Q44" s="18" t="n">
         <v>7</v>
       </c>
       <c r="R44" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S44" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="S44" s="18" t="s">
+      <c r="T44" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="T44" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1719,7 +1715,7 @@
       </c>
       <c r="F47" s="0"/>
       <c r="G47" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I47" s="3" t="n">
         <v>1</v>
@@ -1730,24 +1726,24 @@
       </c>
       <c r="L47" s="0"/>
       <c r="M47" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N47" s="3"/>
       <c r="O47" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P47" s="3"/>
       <c r="Q47" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S47" s="18" t="n">
         <v>74</v>
       </c>
       <c r="T47" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1761,7 +1757,7 @@
       </c>
       <c r="F48" s="0"/>
       <c r="G48" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I48" s="3" t="n">
         <v>0</v>
@@ -1837,7 +1833,7 @@
       </c>
       <c r="F50" s="0"/>
       <c r="G50" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I50" s="19" t="n">
         <v>0</v>
@@ -1936,10 +1932,10 @@
       </c>
       <c r="R52" s="0"/>
       <c r="S52" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="T52" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="T52" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2067,7 +2063,7 @@
       </c>
       <c r="F56" s="0"/>
       <c r="G56" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I56" s="19" t="n">
         <v>0</v>
@@ -2082,7 +2078,7 @@
       </c>
       <c r="N56" s="13"/>
       <c r="O56" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P56" s="3"/>
       <c r="Q56" s="19" t="n">
@@ -2190,7 +2186,7 @@
       </c>
       <c r="N59" s="13"/>
       <c r="O59" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P59" s="3"/>
       <c r="Q59" s="19" t="n">
@@ -2226,7 +2222,7 @@
       </c>
       <c r="N60" s="13"/>
       <c r="O60" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P60" s="3"/>
       <c r="Q60" s="19" t="n">
@@ -2298,7 +2294,7 @@
       </c>
       <c r="N62" s="13"/>
       <c r="O62" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P62" s="3"/>
       <c r="Q62" s="19" t="n">
@@ -2334,7 +2330,7 @@
       </c>
       <c r="N63" s="13"/>
       <c r="O63" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P63" s="3"/>
       <c r="Q63" s="19" t="n">
@@ -2378,10 +2374,10 @@
       </c>
       <c r="R64" s="0"/>
       <c r="S64" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="T64" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="T64" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2415,7 +2411,7 @@
         <v>6</v>
       </c>
       <c r="R65" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S65" s="12" t="n">
         <v>4</v>
@@ -2456,44 +2452,44 @@
         <v>0</v>
       </c>
       <c r="T66" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2"/>
       <c r="C67" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D67" s="0"/>
       <c r="E67" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F67" s="0"/>
       <c r="G67" s="0"/>
       <c r="I67" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J67" s="0"/>
       <c r="K67" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L67" s="0"/>
       <c r="M67" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N67" s="3"/>
       <c r="O67" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P67" s="3"/>
       <c r="Q67" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S67" s="19" t="n">
         <v>0</v>
       </c>
       <c r="T67" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2530,7 +2526,7 @@
         <v>0</v>
       </c>
       <c r="T68" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2557,18 +2553,18 @@
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2"/>
       <c r="C70" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D70" s="0"/>
       <c r="I70" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K70" s="0"/>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
       <c r="P70" s="2"/>
       <c r="Q70" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S70" s="19" t="n">
         <v>0</v>
@@ -2658,7 +2654,7 @@
         <v>5</v>
       </c>
       <c r="T77" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2669,7 +2665,7 @@
       <c r="N78" s="2"/>
       <c r="P78" s="2"/>
       <c r="S78" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2701,7 +2697,7 @@
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="0"/>
       <c r="S82" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2734,127 +2730,127 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Updated documentation for bank up/down information
</commit_message>
<xml_diff>
--- a/Research/Line6_Spider_V_USB_Protocol.xlsx
+++ b/Research/Line6_Spider_V_USB_Protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="112">
   <si>
     <t>Introduction</t>
   </si>
@@ -102,12 +102,30 @@
     <t>ALL INFO 2</t>
   </si>
   <si>
+    <t>ALL INFO 3</t>
+  </si>
+  <si>
+    <t>ALL INFO 4</t>
+  </si>
+  <si>
+    <t>Flood of info once this sent</t>
+  </si>
+  <si>
     <t>PACKET 1 – CONTROL 1</t>
   </si>
   <si>
     <t>PACKET 2 – CONTROL 2</t>
   </si>
   <si>
+    <t>PACKET 1- BANK UP DOWN</t>
+  </si>
+  <si>
+    <t>PACKET 2- BANK UP DOWN</t>
+  </si>
+  <si>
+    <t>Pretty much matches ALL INFO 4 END packet. The amp does send a chunk of data after this, so this is probably a request of data.</t>
+  </si>
+  <si>
     <t>f0</t>
   </si>
   <si>
@@ -141,6 +159,9 @@
     <t>PACKET ## MSB</t>
   </si>
   <si>
+    <t>Always 1</t>
+  </si>
+  <si>
     <t>LSB</t>
   </si>
   <si>
@@ -159,21 +180,27 @@
     <t>Type of message / mode?</t>
   </si>
   <si>
+    <t>0B</t>
+  </si>
+  <si>
+    <t>Bank/Preset Msg</t>
+  </si>
+  <si>
     <t>2D</t>
   </si>
   <si>
     <t>F </t>
   </si>
   <si>
-    <t>0B</t>
-  </si>
-  <si>
     <t>0a </t>
   </si>
   <si>
     <t>Effect on/off command enable?</t>
   </si>
   <si>
+    <t>0D </t>
+  </si>
+  <si>
     <t>2E</t>
   </si>
   <si>
@@ -192,7 +219,16 @@
     <t>3C</t>
   </si>
   <si>
+    <t>Some sort of command end?</t>
+  </si>
+  <si>
     <t>7F</t>
+  </si>
+  <si>
+    <t>0 to 0x7E</t>
+  </si>
+  <si>
+    <t>Preset number</t>
   </si>
   <si>
     <t>7F </t>
@@ -403,7 +439,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,6 +486,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF66FF"/>
         <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0066CC"/>
+        <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF993366"/>
+        <bgColor rgb="FF993366"/>
       </patternFill>
     </fill>
     <fill>
@@ -538,7 +586,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -611,10 +659,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -635,31 +691,63 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -745,10 +833,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T82"/>
+  <dimension ref="A1:X82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P34" activeCellId="0" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -768,7 +856,10 @@
     <col collapsed="false" hidden="false" max="18" min="18" style="2" width="15.1173469387755"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="2" width="19.1224489795918"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="2" width="26.4030612244898"/>
-    <col collapsed="false" hidden="false" max="1023" min="21" style="2" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="26.1887755102041"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="16.2448979591837"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="24.3367346938775"/>
+    <col collapsed="false" hidden="false" max="1023" min="24" style="2" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
@@ -855,6 +946,7 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
       <c r="Q13" s="6"/>
       <c r="S13" s="6"/>
     </row>
@@ -945,10 +1037,27 @@
       <c r="Q26" s="6"/>
       <c r="S26" s="6"/>
     </row>
-    <row r="27" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
+      <c r="D27" s="0"/>
+      <c r="E27" s="0"/>
+      <c r="F27" s="0"/>
+      <c r="G27" s="0"/>
+      <c r="H27" s="0"/>
+      <c r="I27" s="0"/>
+      <c r="J27" s="0"/>
+      <c r="K27" s="0"/>
+      <c r="L27" s="0"/>
+      <c r="M27" s="0"/>
+      <c r="N27" s="0"/>
+      <c r="O27" s="0"/>
+      <c r="P27" s="0"/>
       <c r="Q27" s="6"/>
+      <c r="R27" s="0"/>
       <c r="S27" s="6"/>
+      <c r="T27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
@@ -976,21 +1085,33 @@
       </c>
       <c r="L28" s="9"/>
       <c r="M28" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N28" s="9"/>
       <c r="O28" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="P28" s="9"/>
+        <v>29</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="Q28" s="10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="R28" s="9"/>
       <c r="S28" s="10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="T28" s="0"/>
+      <c r="U28" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="X28" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="n">
@@ -1031,50 +1152,64 @@
         <v>4</v>
       </c>
       <c r="T29" s="0"/>
+      <c r="U29" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="V29" s="1"/>
+      <c r="W29" s="12" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D30" s="0"/>
       <c r="E30" s="14" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F30" s="0"/>
       <c r="G30" s="14" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J30" s="13"/>
       <c r="K30" s="14" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="L30" s="13"/>
       <c r="M30" s="14" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="N30" s="13"/>
       <c r="O30" s="14" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="P30" s="3"/>
       <c r="Q30" s="14" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="R30" s="0"/>
       <c r="S30" s="14" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="T30" s="0"/>
+      <c r="U30" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="V30" s="1"/>
+      <c r="W30" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C31" s="14" t="n">
         <v>0</v>
@@ -1111,10 +1246,17 @@
         <v>0</v>
       </c>
       <c r="T31" s="0"/>
+      <c r="U31" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="V31" s="1"/>
+      <c r="W31" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C32" s="14" t="n">
         <v>1</v>
@@ -1151,6 +1293,13 @@
         <v>1</v>
       </c>
       <c r="T32" s="0"/>
+      <c r="U32" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="V32" s="1"/>
+      <c r="W32" s="14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -1191,46 +1340,60 @@
         <v>4</v>
       </c>
       <c r="T33" s="0"/>
+      <c r="U33" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="V33" s="1"/>
+      <c r="W33" s="12" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D34" s="0"/>
       <c r="E34" s="14" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F34" s="0"/>
       <c r="G34" s="14" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="J34" s="13"/>
       <c r="K34" s="14" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="L34" s="13"/>
       <c r="M34" s="14" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="N34" s="13"/>
       <c r="O34" s="14" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="P34" s="3"/>
       <c r="Q34" s="14" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="R34" s="0"/>
       <c r="S34" s="14" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="T34" s="0"/>
+      <c r="U34" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="V34" s="1"/>
+      <c r="W34" s="14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
@@ -1271,10 +1434,17 @@
         <v>22</v>
       </c>
       <c r="T35" s="0"/>
+      <c r="U35" s="14" t="n">
+        <v>22</v>
+      </c>
+      <c r="V35" s="1"/>
+      <c r="W35" s="14" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C36" s="14" t="n">
         <v>0</v>
@@ -1311,6 +1481,13 @@
         <v>0</v>
       </c>
       <c r="T36" s="0"/>
+      <c r="U36" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="V36" s="1"/>
+      <c r="W36" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="15"/>
@@ -1349,47 +1526,66 @@
         <v>4</v>
       </c>
       <c r="T37" s="0"/>
+      <c r="U37" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="V37" s="1"/>
+      <c r="W37" s="12" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D38" s="0"/>
       <c r="E38" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F38" s="0"/>
       <c r="G38" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="J38" s="13"/>
       <c r="K38" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="L38" s="13"/>
       <c r="M38" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="N38" s="13"/>
       <c r="O38" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="P38" s="3"/>
       <c r="Q38" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="R38" s="0"/>
       <c r="S38" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="T38" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="U38" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="V38" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="W38" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="X38" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1422,14 +1618,26 @@
       </c>
       <c r="P39" s="3"/>
       <c r="Q39" s="16" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="R39" s="0"/>
       <c r="S39" s="16" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
+      </c>
+      <c r="U39" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="V39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W39" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="X39" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1462,14 +1670,26 @@
       </c>
       <c r="P40" s="3"/>
       <c r="Q40" s="16" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="R40" s="0"/>
       <c r="S40" s="16" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="U40" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="V40" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="W40" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="X40" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,6 +1729,13 @@
         <v>4</v>
       </c>
       <c r="T41" s="0"/>
+      <c r="U41" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="V41" s="1"/>
+      <c r="W41" s="12" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
@@ -1539,14 +1766,21 @@
         <v>0</v>
       </c>
       <c r="P42" s="3"/>
-      <c r="Q42" s="18" t="n">
+      <c r="Q42" s="19" t="n">
         <v>0</v>
       </c>
       <c r="R42" s="0"/>
-      <c r="S42" s="18" t="n">
+      <c r="S42" s="19" t="n">
         <v>0</v>
       </c>
       <c r="T42" s="0"/>
+      <c r="U42" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V42" s="1"/>
+      <c r="W42" s="20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
@@ -1577,14 +1811,21 @@
         <v>0</v>
       </c>
       <c r="P43" s="3"/>
-      <c r="Q43" s="18" t="n">
+      <c r="Q43" s="19" t="n">
         <v>0</v>
       </c>
       <c r="R43" s="0"/>
-      <c r="S43" s="18" t="n">
+      <c r="S43" s="19" t="n">
         <v>0</v>
       </c>
       <c r="T43" s="0"/>
+      <c r="U43" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V43" s="1"/>
+      <c r="W43" s="20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2"/>
@@ -1612,20 +1853,29 @@
       </c>
       <c r="N44" s="3"/>
       <c r="O44" s="3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="P44" s="3"/>
-      <c r="Q44" s="18" t="n">
+      <c r="Q44" s="19" t="n">
         <v>7</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="S44" s="18" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="S44" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
+      </c>
+      <c r="U44" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="V44" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W44" s="20" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,6 +1915,13 @@
         <v>4</v>
       </c>
       <c r="T45" s="0"/>
+      <c r="U45" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="V45" s="1"/>
+      <c r="W45" s="12" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
@@ -1695,14 +1952,21 @@
         <v>0</v>
       </c>
       <c r="P46" s="3"/>
-      <c r="Q46" s="18" t="n">
+      <c r="Q46" s="19" t="n">
         <v>0</v>
       </c>
       <c r="R46" s="0"/>
-      <c r="S46" s="18" t="n">
+      <c r="S46" s="19" t="n">
         <v>0</v>
       </c>
       <c r="T46" s="0"/>
+      <c r="U46" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V46" s="1"/>
+      <c r="W46" s="20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0"/>
@@ -1715,7 +1979,7 @@
       </c>
       <c r="F47" s="0"/>
       <c r="G47" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="I47" s="3" t="n">
         <v>1</v>
@@ -1726,24 +1990,33 @@
       </c>
       <c r="L47" s="0"/>
       <c r="M47" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="N47" s="3"/>
       <c r="O47" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P47" s="3"/>
-      <c r="Q47" s="18" t="s">
+      <c r="Q47" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="R47" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S47" s="19" t="n">
+        <v>74</v>
+      </c>
+      <c r="T47" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="U47" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="V47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W47" s="20" t="s">
         <v>50</v>
-      </c>
-      <c r="R47" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="S47" s="18" t="n">
-        <v>74</v>
-      </c>
-      <c r="T47" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1757,7 +2030,7 @@
       </c>
       <c r="F48" s="0"/>
       <c r="G48" s="3" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="I48" s="3" t="n">
         <v>0</v>
@@ -1775,14 +2048,21 @@
         <v>0</v>
       </c>
       <c r="P48" s="3"/>
-      <c r="Q48" s="18" t="n">
+      <c r="Q48" s="19" t="n">
         <v>0</v>
       </c>
       <c r="R48" s="0"/>
-      <c r="S48" s="18" t="n">
+      <c r="S48" s="19" t="n">
         <v>3</v>
       </c>
       <c r="T48" s="0"/>
+      <c r="U48" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V48" s="1"/>
+      <c r="W48" s="20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
@@ -1821,10 +2101,17 @@
         <v>4</v>
       </c>
       <c r="T49" s="0"/>
+      <c r="U49" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="V49" s="1"/>
+      <c r="W49" s="12" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
-      <c r="C50" s="19" t="n">
+      <c r="C50" s="21" t="n">
         <v>0</v>
       </c>
       <c r="D50" s="0"/>
@@ -1833,17 +2120,17 @@
       </c>
       <c r="F50" s="0"/>
       <c r="G50" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I50" s="19" t="n">
+        <v>62</v>
+      </c>
+      <c r="I50" s="21" t="n">
         <v>0</v>
       </c>
       <c r="J50" s="13"/>
-      <c r="K50" s="19" t="n">
+      <c r="K50" s="21" t="n">
         <v>0</v>
       </c>
       <c r="L50" s="13"/>
-      <c r="M50" s="19" t="n">
+      <c r="M50" s="21" t="n">
         <v>0</v>
       </c>
       <c r="N50" s="13"/>
@@ -1851,18 +2138,25 @@
         <v>0</v>
       </c>
       <c r="P50" s="3"/>
-      <c r="Q50" s="18" t="n">
+      <c r="Q50" s="19" t="n">
         <v>0</v>
       </c>
       <c r="R50" s="0"/>
-      <c r="S50" s="18" t="n">
+      <c r="S50" s="19" t="n">
         <v>0</v>
       </c>
       <c r="T50" s="0"/>
+      <c r="U50" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V50" s="1"/>
+      <c r="W50" s="20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
-      <c r="C51" s="19" t="n">
+      <c r="C51" s="21" t="n">
         <v>0</v>
       </c>
       <c r="D51" s="0"/>
@@ -1873,15 +2167,15 @@
       <c r="G51" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="I51" s="19" t="n">
+      <c r="I51" s="21" t="n">
         <v>0</v>
       </c>
       <c r="J51" s="13"/>
-      <c r="K51" s="19" t="n">
+      <c r="K51" s="21" t="n">
         <v>0</v>
       </c>
       <c r="L51" s="13"/>
-      <c r="M51" s="19" t="n">
+      <c r="M51" s="21" t="n">
         <v>0</v>
       </c>
       <c r="N51" s="13"/>
@@ -1889,18 +2183,25 @@
         <v>0</v>
       </c>
       <c r="P51" s="3"/>
-      <c r="Q51" s="18" t="n">
+      <c r="Q51" s="19" t="n">
         <v>0</v>
       </c>
       <c r="R51" s="0"/>
-      <c r="S51" s="18" t="n">
+      <c r="S51" s="19" t="n">
         <v>0</v>
       </c>
       <c r="T51" s="0"/>
+      <c r="U51" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V51" s="1"/>
+      <c r="W51" s="20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0"/>
-      <c r="C52" s="19" t="n">
+      <c r="C52" s="21" t="n">
         <v>0</v>
       </c>
       <c r="D52" s="0"/>
@@ -1911,15 +2212,15 @@
       <c r="G52" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I52" s="19" t="n">
+      <c r="I52" s="21" t="n">
         <v>0</v>
       </c>
       <c r="J52" s="13"/>
-      <c r="K52" s="19" t="n">
+      <c r="K52" s="21" t="n">
         <v>0</v>
       </c>
       <c r="L52" s="13"/>
-      <c r="M52" s="19" t="n">
+      <c r="M52" s="21" t="n">
         <v>0</v>
       </c>
       <c r="N52" s="13"/>
@@ -1927,15 +2228,22 @@
         <v>4</v>
       </c>
       <c r="P52" s="3"/>
-      <c r="Q52" s="18" t="n">
+      <c r="Q52" s="19" t="n">
         <v>10</v>
       </c>
       <c r="R52" s="0"/>
-      <c r="S52" s="20" t="s">
-        <v>54</v>
+      <c r="S52" s="22" t="s">
+        <v>63</v>
       </c>
       <c r="T52" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
+      </c>
+      <c r="U52" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="V52" s="1"/>
+      <c r="W52" s="20" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1948,7 +2256,7 @@
         <v>4</v>
       </c>
       <c r="F53" s="0"/>
-      <c r="G53" s="21" t="n">
+      <c r="G53" s="23" t="n">
         <v>7</v>
       </c>
       <c r="I53" s="12" t="n">
@@ -1975,29 +2283,36 @@
         <v>4</v>
       </c>
       <c r="T53" s="0"/>
+      <c r="U53" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="V53" s="1"/>
+      <c r="W53" s="12" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0"/>
-      <c r="C54" s="19" t="n">
+      <c r="C54" s="21" t="n">
         <v>0</v>
       </c>
       <c r="D54" s="0"/>
-      <c r="E54" s="19" t="n">
+      <c r="E54" s="21" t="n">
         <v>0</v>
       </c>
       <c r="F54" s="0"/>
-      <c r="G54" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="I54" s="19" t="n">
+      <c r="G54" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" s="21" t="n">
         <v>0</v>
       </c>
       <c r="J54" s="13"/>
-      <c r="K54" s="19" t="n">
+      <c r="K54" s="21" t="n">
         <v>0</v>
       </c>
       <c r="L54" s="13"/>
-      <c r="M54" s="19" t="n">
+      <c r="M54" s="21" t="n">
         <v>0</v>
       </c>
       <c r="N54" s="13"/>
@@ -2005,37 +2320,44 @@
         <v>0</v>
       </c>
       <c r="P54" s="3"/>
-      <c r="Q54" s="19" t="n">
+      <c r="Q54" s="21" t="n">
         <v>0</v>
       </c>
       <c r="R54" s="0"/>
-      <c r="S54" s="18" t="n">
+      <c r="S54" s="19" t="n">
         <v>3</v>
       </c>
       <c r="T54" s="0"/>
+      <c r="U54" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V54" s="1"/>
+      <c r="W54" s="20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2"/>
-      <c r="C55" s="19" t="n">
+      <c r="C55" s="21" t="n">
         <v>0</v>
       </c>
       <c r="D55" s="0"/>
-      <c r="E55" s="19" t="n">
+      <c r="E55" s="21" t="n">
         <v>0</v>
       </c>
       <c r="F55" s="0"/>
-      <c r="G55" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="I55" s="19" t="n">
+      <c r="G55" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" s="21" t="n">
         <v>0</v>
       </c>
       <c r="J55" s="13"/>
-      <c r="K55" s="19" t="n">
+      <c r="K55" s="21" t="n">
         <v>0</v>
       </c>
       <c r="L55" s="13"/>
-      <c r="M55" s="19" t="n">
+      <c r="M55" s="21" t="n">
         <v>0</v>
       </c>
       <c r="N55" s="13"/>
@@ -2043,52 +2365,66 @@
         <v>0</v>
       </c>
       <c r="P55" s="3"/>
-      <c r="Q55" s="19" t="n">
+      <c r="Q55" s="21" t="n">
         <v>0</v>
       </c>
       <c r="R55" s="0"/>
-      <c r="S55" s="18" t="n">
+      <c r="S55" s="19" t="n">
         <v>0</v>
       </c>
       <c r="T55" s="0"/>
+      <c r="U55" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V55" s="1"/>
+      <c r="W55" s="20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2"/>
-      <c r="C56" s="19" t="n">
+      <c r="C56" s="21" t="n">
         <v>0</v>
       </c>
       <c r="D56" s="0"/>
-      <c r="E56" s="19" t="n">
+      <c r="E56" s="21" t="n">
         <v>0</v>
       </c>
       <c r="F56" s="0"/>
-      <c r="G56" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="I56" s="19" t="n">
+      <c r="G56" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="I56" s="21" t="n">
         <v>0</v>
       </c>
       <c r="J56" s="13"/>
-      <c r="K56" s="19" t="n">
+      <c r="K56" s="21" t="n">
         <v>0</v>
       </c>
       <c r="L56" s="13"/>
-      <c r="M56" s="19" t="n">
+      <c r="M56" s="21" t="n">
         <v>0</v>
       </c>
       <c r="N56" s="13"/>
       <c r="O56" s="3" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="P56" s="3"/>
-      <c r="Q56" s="19" t="n">
+      <c r="Q56" s="21" t="n">
         <v>0</v>
       </c>
       <c r="R56" s="0"/>
-      <c r="S56" s="18" t="n">
+      <c r="S56" s="19" t="n">
         <v>0</v>
       </c>
       <c r="T56" s="0"/>
+      <c r="U56" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V56" s="1"/>
+      <c r="W56" s="20" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2"/>
@@ -2113,7 +2449,7 @@
         <v>4</v>
       </c>
       <c r="N57" s="13"/>
-      <c r="O57" s="12" t="n">
+      <c r="O57" s="26" t="n">
         <v>4</v>
       </c>
       <c r="P57" s="3"/>
@@ -2125,114 +2461,147 @@
         <v>4</v>
       </c>
       <c r="T57" s="0"/>
+      <c r="U57" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="V57" s="1"/>
+      <c r="W57" s="26" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2"/>
-      <c r="C58" s="19" t="n">
+      <c r="C58" s="21" t="n">
         <v>0</v>
       </c>
       <c r="D58" s="0"/>
-      <c r="E58" s="19" t="n">
+      <c r="E58" s="21" t="n">
         <v>0</v>
       </c>
       <c r="F58" s="0"/>
       <c r="G58" s="0"/>
-      <c r="I58" s="19" t="n">
+      <c r="I58" s="21" t="n">
         <v>0</v>
       </c>
       <c r="J58" s="13"/>
-      <c r="K58" s="19" t="n">
+      <c r="K58" s="21" t="n">
         <v>0</v>
       </c>
       <c r="L58" s="13"/>
-      <c r="M58" s="19" t="n">
+      <c r="M58" s="21" t="n">
         <v>0</v>
       </c>
       <c r="N58" s="13"/>
-      <c r="O58" s="3" t="n">
+      <c r="O58" s="27" t="n">
         <v>0</v>
       </c>
       <c r="P58" s="3"/>
-      <c r="Q58" s="19" t="n">
+      <c r="Q58" s="21" t="n">
         <v>0</v>
       </c>
       <c r="R58" s="0"/>
-      <c r="S58" s="18" t="n">
+      <c r="S58" s="19" t="n">
         <v>0</v>
       </c>
       <c r="T58" s="0"/>
+      <c r="U58" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="V58" s="1"/>
+      <c r="W58" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="X58" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2"/>
-      <c r="C59" s="19" t="n">
+      <c r="C59" s="21" t="n">
         <v>0</v>
       </c>
       <c r="D59" s="0"/>
-      <c r="E59" s="19" t="n">
+      <c r="E59" s="21" t="n">
         <v>0</v>
       </c>
       <c r="F59" s="0"/>
       <c r="G59" s="0"/>
-      <c r="I59" s="19" t="n">
+      <c r="I59" s="21" t="n">
         <v>0</v>
       </c>
       <c r="J59" s="13"/>
-      <c r="K59" s="19" t="n">
+      <c r="K59" s="21" t="n">
         <v>0</v>
       </c>
       <c r="L59" s="13"/>
-      <c r="M59" s="19" t="n">
+      <c r="M59" s="21" t="n">
         <v>0</v>
       </c>
       <c r="N59" s="13"/>
-      <c r="O59" s="3" t="s">
-        <v>58</v>
+      <c r="O59" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="P59" s="3"/>
-      <c r="Q59" s="19" t="n">
+      <c r="Q59" s="21" t="n">
         <v>0</v>
       </c>
       <c r="R59" s="0"/>
-      <c r="S59" s="18" t="n">
+      <c r="S59" s="19" t="n">
         <v>3</v>
       </c>
       <c r="T59" s="0"/>
+      <c r="U59" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="V59" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="W59" s="29" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2"/>
-      <c r="C60" s="19" t="n">
+      <c r="C60" s="21" t="n">
         <v>0</v>
       </c>
       <c r="D60" s="0"/>
-      <c r="E60" s="19" t="n">
+      <c r="E60" s="21" t="n">
         <v>0</v>
       </c>
       <c r="F60" s="0"/>
       <c r="G60" s="0"/>
-      <c r="I60" s="19" t="n">
+      <c r="I60" s="21" t="n">
         <v>0</v>
       </c>
       <c r="J60" s="13"/>
-      <c r="K60" s="19" t="n">
+      <c r="K60" s="21" t="n">
         <v>0</v>
       </c>
       <c r="L60" s="13"/>
-      <c r="M60" s="19" t="n">
+      <c r="M60" s="21" t="n">
         <v>0</v>
       </c>
       <c r="N60" s="13"/>
-      <c r="O60" s="3" t="s">
-        <v>59</v>
+      <c r="O60" s="27" t="s">
+        <v>71</v>
       </c>
       <c r="P60" s="3"/>
-      <c r="Q60" s="19" t="n">
+      <c r="Q60" s="21" t="n">
         <v>0</v>
       </c>
       <c r="R60" s="0"/>
-      <c r="S60" s="18" t="n">
+      <c r="S60" s="19" t="n">
         <v>0</v>
       </c>
       <c r="T60" s="0"/>
+      <c r="U60" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="V60" s="1"/>
+      <c r="W60" s="29" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2"/>
@@ -2257,7 +2626,7 @@
         <v>4</v>
       </c>
       <c r="N61" s="13"/>
-      <c r="O61" s="12" t="n">
+      <c r="O61" s="30" t="n">
         <v>4</v>
       </c>
       <c r="P61" s="3"/>
@@ -2269,304 +2638,358 @@
         <v>4</v>
       </c>
       <c r="T61" s="0"/>
+      <c r="U61" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="V61" s="1"/>
+      <c r="W61" s="30" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2"/>
-      <c r="C62" s="19" t="n">
+      <c r="C62" s="21" t="n">
         <v>0</v>
       </c>
       <c r="D62" s="0"/>
-      <c r="E62" s="19" t="n">
+      <c r="E62" s="21" t="n">
         <v>0</v>
       </c>
       <c r="F62" s="0"/>
       <c r="G62" s="0"/>
-      <c r="I62" s="19" t="n">
+      <c r="I62" s="21" t="n">
         <v>0</v>
       </c>
       <c r="J62" s="13"/>
-      <c r="K62" s="19" t="n">
+      <c r="K62" s="21" t="n">
         <v>0</v>
       </c>
       <c r="L62" s="13"/>
-      <c r="M62" s="19" t="n">
+      <c r="M62" s="21" t="n">
         <v>0</v>
       </c>
       <c r="N62" s="13"/>
-      <c r="O62" s="3" t="s">
-        <v>58</v>
+      <c r="O62" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="P62" s="3"/>
-      <c r="Q62" s="19" t="n">
+      <c r="Q62" s="21" t="n">
         <v>0</v>
       </c>
       <c r="R62" s="0"/>
-      <c r="S62" s="18" t="n">
+      <c r="S62" s="19" t="n">
         <v>0</v>
       </c>
       <c r="T62" s="0"/>
+      <c r="U62" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V62" s="1"/>
+      <c r="W62" s="29" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
-      <c r="C63" s="19" t="n">
+      <c r="C63" s="21" t="n">
         <v>0</v>
       </c>
       <c r="D63" s="0"/>
-      <c r="E63" s="19" t="n">
+      <c r="E63" s="21" t="n">
         <v>0</v>
       </c>
       <c r="F63" s="0"/>
       <c r="G63" s="0"/>
-      <c r="I63" s="19" t="n">
+      <c r="I63" s="21" t="n">
         <v>0</v>
       </c>
       <c r="J63" s="13"/>
-      <c r="K63" s="19" t="n">
+      <c r="K63" s="21" t="n">
         <v>0</v>
       </c>
       <c r="L63" s="13"/>
-      <c r="M63" s="19" t="n">
+      <c r="M63" s="21" t="n">
         <v>0</v>
       </c>
       <c r="N63" s="13"/>
-      <c r="O63" s="3" t="s">
-        <v>58</v>
+      <c r="O63" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="P63" s="3"/>
-      <c r="Q63" s="19" t="n">
+      <c r="Q63" s="21" t="n">
         <v>0</v>
       </c>
       <c r="R63" s="0"/>
-      <c r="S63" s="18" t="n">
+      <c r="S63" s="19" t="n">
         <v>0</v>
       </c>
       <c r="T63" s="0"/>
+      <c r="U63" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V63" s="1"/>
+      <c r="W63" s="29" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
-      <c r="C64" s="19" t="n">
+      <c r="C64" s="21" t="n">
         <v>0</v>
       </c>
       <c r="D64" s="0"/>
-      <c r="E64" s="19" t="n">
+      <c r="E64" s="21" t="n">
         <v>0</v>
       </c>
       <c r="F64" s="0"/>
       <c r="G64" s="0"/>
-      <c r="I64" s="19" t="n">
+      <c r="I64" s="21" t="n">
         <v>0</v>
       </c>
       <c r="J64" s="13"/>
-      <c r="K64" s="19" t="n">
+      <c r="K64" s="21" t="n">
         <v>0</v>
       </c>
       <c r="L64" s="13"/>
-      <c r="M64" s="19" t="n">
+      <c r="M64" s="21" t="n">
         <v>0</v>
       </c>
       <c r="N64" s="13"/>
-      <c r="O64" s="3" t="n">
+      <c r="O64" s="31" t="n">
         <v>0</v>
       </c>
       <c r="P64" s="3"/>
-      <c r="Q64" s="19" t="n">
+      <c r="Q64" s="21" t="n">
         <v>0</v>
       </c>
       <c r="R64" s="0"/>
-      <c r="S64" s="20" t="s">
-        <v>60</v>
+      <c r="S64" s="22" t="s">
+        <v>72</v>
       </c>
       <c r="T64" s="2" t="s">
-        <v>61</v>
+        <v>73</v>
+      </c>
+      <c r="U64" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V64" s="1"/>
+      <c r="W64" s="32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2"/>
-      <c r="C65" s="24" t="n">
+      <c r="C65" s="33" t="n">
         <v>6</v>
       </c>
       <c r="D65" s="0"/>
-      <c r="E65" s="24" t="n">
+      <c r="E65" s="33" t="n">
         <v>6</v>
       </c>
       <c r="F65" s="0"/>
       <c r="G65" s="0"/>
-      <c r="I65" s="24" t="n">
+      <c r="I65" s="33" t="n">
         <v>6</v>
       </c>
       <c r="J65" s="0"/>
-      <c r="K65" s="24" t="n">
+      <c r="K65" s="33" t="n">
         <v>6</v>
       </c>
       <c r="L65" s="0"/>
-      <c r="M65" s="24" t="n">
+      <c r="M65" s="33" t="n">
         <v>6</v>
       </c>
       <c r="N65" s="3"/>
-      <c r="O65" s="24" t="n">
+      <c r="O65" s="33" t="n">
         <v>6</v>
       </c>
       <c r="P65" s="3"/>
-      <c r="Q65" s="24" t="n">
+      <c r="Q65" s="33" t="n">
         <v>6</v>
       </c>
       <c r="R65" s="2" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="S65" s="12" t="n">
         <v>4</v>
       </c>
       <c r="T65" s="0"/>
+      <c r="U65" s="33" t="n">
+        <v>6</v>
+      </c>
+      <c r="W65" s="33" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2"/>
-      <c r="C66" s="25" t="n">
+      <c r="C66" s="34" t="n">
         <v>0</v>
       </c>
       <c r="D66" s="0"/>
-      <c r="E66" s="25" t="n">
+      <c r="E66" s="34" t="n">
         <v>0</v>
       </c>
       <c r="F66" s="0"/>
       <c r="G66" s="0"/>
-      <c r="I66" s="25" t="n">
+      <c r="I66" s="34" t="n">
         <v>0</v>
       </c>
       <c r="J66" s="0"/>
-      <c r="K66" s="25" t="n">
+      <c r="K66" s="34" t="n">
         <v>0</v>
       </c>
       <c r="L66" s="0"/>
-      <c r="M66" s="25" t="n">
+      <c r="M66" s="34" t="n">
         <v>0</v>
       </c>
       <c r="N66" s="3"/>
-      <c r="O66" s="25" t="n">
+      <c r="O66" s="34" t="n">
         <v>0</v>
       </c>
       <c r="P66" s="3"/>
-      <c r="Q66" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="S66" s="19" t="n">
+      <c r="Q66" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="S66" s="21" t="n">
         <v>0</v>
       </c>
       <c r="T66" s="2" t="s">
-        <v>63</v>
+        <v>75</v>
+      </c>
+      <c r="U66" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="W66" s="34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2"/>
-      <c r="C67" s="25" t="s">
-        <v>56</v>
+      <c r="C67" s="34" t="s">
+        <v>65</v>
       </c>
       <c r="D67" s="0"/>
-      <c r="E67" s="25" t="s">
-        <v>56</v>
+      <c r="E67" s="34" t="s">
+        <v>65</v>
       </c>
       <c r="F67" s="0"/>
       <c r="G67" s="0"/>
-      <c r="I67" s="25" t="s">
-        <v>56</v>
+      <c r="I67" s="34" t="s">
+        <v>65</v>
       </c>
       <c r="J67" s="0"/>
-      <c r="K67" s="25" t="s">
-        <v>56</v>
+      <c r="K67" s="34" t="s">
+        <v>65</v>
       </c>
       <c r="L67" s="0"/>
-      <c r="M67" s="25" t="s">
-        <v>56</v>
+      <c r="M67" s="34" t="s">
+        <v>65</v>
       </c>
       <c r="N67" s="3"/>
-      <c r="O67" s="25" t="s">
-        <v>56</v>
+      <c r="O67" s="34" t="s">
+        <v>65</v>
       </c>
       <c r="P67" s="3"/>
-      <c r="Q67" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="S67" s="19" t="n">
+      <c r="Q67" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="S67" s="21" t="n">
         <v>0</v>
       </c>
       <c r="T67" s="2" t="s">
-        <v>64</v>
+        <v>76</v>
+      </c>
+      <c r="U67" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="W67" s="34" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2"/>
-      <c r="C68" s="26" t="n">
+      <c r="C68" s="35" t="n">
         <v>0</v>
       </c>
       <c r="D68" s="0"/>
-      <c r="E68" s="26" t="n">
+      <c r="E68" s="35" t="n">
         <v>0</v>
       </c>
       <c r="F68" s="0"/>
       <c r="G68" s="0"/>
-      <c r="I68" s="26" t="n">
+      <c r="I68" s="35" t="n">
         <v>0</v>
       </c>
       <c r="J68" s="0"/>
-      <c r="K68" s="26" t="n">
+      <c r="K68" s="35" t="n">
         <v>0</v>
       </c>
       <c r="L68" s="0"/>
-      <c r="M68" s="26" t="n">
+      <c r="M68" s="35" t="n">
         <v>0</v>
       </c>
       <c r="N68" s="3"/>
-      <c r="O68" s="26" t="n">
+      <c r="O68" s="35" t="n">
         <v>0</v>
       </c>
       <c r="P68" s="3"/>
-      <c r="Q68" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="S68" s="19" t="n">
+      <c r="Q68" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="S68" s="21" t="n">
         <v>0</v>
       </c>
       <c r="T68" s="2" t="s">
-        <v>64</v>
+        <v>76</v>
+      </c>
+      <c r="U68" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="W68" s="35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2"/>
-      <c r="C69" s="27"/>
+      <c r="C69" s="36"/>
       <c r="D69" s="15"/>
       <c r="E69" s="15"/>
       <c r="F69" s="15"/>
-      <c r="G69" s="27"/>
-      <c r="I69" s="27"/>
-      <c r="J69" s="27"/>
-      <c r="K69" s="27"/>
-      <c r="L69" s="27"/>
+      <c r="G69" s="36"/>
+      <c r="I69" s="36"/>
+      <c r="J69" s="36"/>
+      <c r="K69" s="36"/>
+      <c r="L69" s="36"/>
       <c r="M69" s="15"/>
       <c r="N69" s="15"/>
-      <c r="O69" s="27"/>
+      <c r="O69" s="36"/>
       <c r="P69" s="2"/>
       <c r="Q69" s="15"/>
       <c r="S69" s="12" t="n">
         <v>4</v>
       </c>
       <c r="T69" s="0"/>
+      <c r="U69" s="15"/>
+      <c r="W69" s="37"/>
     </row>
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2"/>
       <c r="C70" s="0" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D70" s="0"/>
       <c r="I70" s="5" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="K70" s="0"/>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
       <c r="P70" s="2"/>
       <c r="Q70" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S70" s="19" t="n">
+        <v>79</v>
+      </c>
+      <c r="S70" s="21" t="n">
         <v>0</v>
       </c>
       <c r="T70" s="0"/>
@@ -2578,7 +3001,7 @@
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
       <c r="P71" s="2"/>
-      <c r="S71" s="19" t="n">
+      <c r="S71" s="21" t="n">
         <v>0</v>
       </c>
       <c r="T71" s="0"/>
@@ -2590,7 +3013,7 @@
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="P72" s="2"/>
-      <c r="S72" s="19" t="n">
+      <c r="S72" s="21" t="n">
         <v>0</v>
       </c>
       <c r="T72" s="0"/>
@@ -2614,7 +3037,7 @@
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
       <c r="P74" s="2"/>
-      <c r="S74" s="19" t="n">
+      <c r="S74" s="21" t="n">
         <v>0</v>
       </c>
       <c r="T74" s="0"/>
@@ -2626,7 +3049,7 @@
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="P75" s="2"/>
-      <c r="S75" s="19" t="n">
+      <c r="S75" s="21" t="n">
         <v>0</v>
       </c>
       <c r="T75" s="0"/>
@@ -2638,7 +3061,7 @@
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
       <c r="P76" s="2"/>
-      <c r="S76" s="19" t="n">
+      <c r="S76" s="21" t="n">
         <v>0</v>
       </c>
       <c r="T76" s="0"/>
@@ -2650,11 +3073,11 @@
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
       <c r="P77" s="2"/>
-      <c r="S77" s="28" t="n">
+      <c r="S77" s="38" t="n">
         <v>5</v>
       </c>
       <c r="T77" s="2" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2664,8 +3087,8 @@
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
       <c r="P78" s="2"/>
-      <c r="S78" s="29" t="s">
-        <v>69</v>
+      <c r="S78" s="39" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2675,7 +3098,7 @@
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
       <c r="P79" s="2"/>
-      <c r="S79" s="29" t="n">
+      <c r="S79" s="39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2686,7 +3109,7 @@
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
       <c r="P80" s="2"/>
-      <c r="S80" s="30" t="n">
+      <c r="S80" s="40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2697,7 +3120,7 @@
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="0"/>
       <c r="S82" s="2" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2718,7 +3141,7 @@
   </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -2729,128 +3152,128 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31" t="s">
-        <v>55</v>
+      <c r="A1" s="41" t="s">
+        <v>64</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>